<commit_message>
fixed the class list wont have duplicates alr
</commit_message>
<xml_diff>
--- a/Class List.xlsx
+++ b/Class List.xlsx
@@ -14,7 +14,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <x:si>
+    <x:t>STF_ENG, Abelanes Maria Teresa Robles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Module Leader</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Azhar Bin Moh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LMS TSO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Chow Kok Peng</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Ho Kuan Tat Jackson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Low Poh Lian</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lecturer (Teaching Team)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Lye Sau Lin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Tan Geok Ling</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Wee May Lin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Yan Seow Chiang</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STF_ENG, Yeo Sock Kiang May</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, ANG JIA JUN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Learner</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, CHIM JUN XI LEROY GABRIEL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, DHANI ARJUNA PUTRA BIN SHAZALI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, HUAN JIAX CHOU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, JASON PHUA KAI XIANG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, JOHNSON NG CHONG SHENG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, KALLANAYAKANAHALLI KANISHK PRABHAKAR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, LI HAOYANG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, MAHAESWAR S/O RAJENDRA PRASAD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, MOWER PRISCILLA LE XUAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, MUHAMMAD ILHAM GONZAGA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, PANG ZI JIAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, SOH WEI QUAN ROYDON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, TAN KE MING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, TEO YONG JIE ASHER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, VINAYA SENTHILKUMAR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, WANG PENGYU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, WANG RUI ZHE EDDRICK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, YONG KAH HAO MARCUS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, YUSUF RAMI NAZZAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, ZAW YE YINT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STU_ENG, ZHANG RAN</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,7 +477,264 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="B1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="B2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="B3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="B4" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="B5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="B6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="B7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="B8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3">
+      <x:c r="B9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3">
+      <x:c r="B10" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3">
+      <x:c r="B11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:3">
+      <x:c r="B12" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:3">
+      <x:c r="B13" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:3">
+      <x:c r="B14" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:3">
+      <x:c r="B15" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3">
+      <x:c r="B16" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3">
+      <x:c r="B17" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:3">
+      <x:c r="B18" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:3">
+      <x:c r="B19" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:3">
+      <x:c r="B20" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:3">
+      <x:c r="B21" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:3">
+      <x:c r="B22" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:3">
+      <x:c r="B23" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:3">
+      <x:c r="B24" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:3">
+      <x:c r="B25" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:3">
+      <x:c r="B26" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:3">
+      <x:c r="B27" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:3">
+      <x:c r="B28" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:3">
+      <x:c r="B29" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:3">
+      <x:c r="B30" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:3">
+      <x:c r="B31" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:3">
+      <x:c r="B32" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>